<commit_message>
continued to improve on zooplankton models, added predictions for x2
</commit_message>
<xml_diff>
--- a/data/Biomass conversions.xlsx
+++ b/data/Biomass conversions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\ZoopSynth\Data paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/salinity control gates/SFHA_synthesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E8C096-A92A-4650-89A0-C853302FCD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{53E8C096-A92A-4650-89A0-C853302FCD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EC79986-BA84-4E5C-99F7-CAB287F07D59}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Micro and Meso-zooplankton" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="92">
   <si>
     <t>Taxname</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>CDFW, unpublished</t>
+  </si>
+  <si>
+    <t>Eurytemora carolleeae</t>
   </si>
 </sst>
 </file>
@@ -430,10 +433,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -441,31 +444,19 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -475,7 +466,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -762,24 +752,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13C544B-28E0-4ED3-8459-C8F5B3BB063B}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46:A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="3"/>
+    <col min="3" max="3" width="13.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="3" customWidth="1"/>
-    <col min="5" max="5" width="213" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="213" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,756 +782,807 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="5">
         <v>3.36</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="4">
         <v>2.984</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4">
         <v>1.3009999999999999</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4">
         <v>2.6659999999999999</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="5">
         <v>1.1619999999999999</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="C7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7">
         <v>0.3</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="5">
         <v>0.6</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="9">
+      <c r="C9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7">
         <v>3</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="3">
         <v>1.5</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="5">
         <v>3.8</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="9">
+      <c r="C12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="3">
         <v>3.36</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="3">
         <v>1.68</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="5">
         <v>4</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="5">
         <v>1</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="5">
         <v>4</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="5">
         <v>2</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="10">
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5">
         <v>3.55</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="5">
         <v>1.4430000000000001</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="5">
         <v>0.1</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="9">
+      <c r="C23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="7">
         <v>0.04</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="10">
+      <c r="C24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="5">
         <v>0.13300000000000001</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="7">
         <v>0.04</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="5">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="10">
+      <c r="B27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5">
         <v>0.13300000000000001</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="10">
+      <c r="B28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="5">
         <v>8.8663036902600939E-2</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="5">
         <v>0.04</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="5">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="5">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="10">
+      <c r="B32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="5">
         <v>0.21</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="16">
+      <c r="B33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="10">
         <v>0.5</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="9">
+      <c r="C34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="5">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D36" s="5">
         <v>0.1</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="10">
+      <c r="B37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="5">
         <v>2.6619999999999999</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="7" t="s">
+      <c r="B38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="7" t="s">
+      <c r="B40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="5">
         <v>3.4129999999999998</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="7" t="s">
+      <c r="B41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="5">
         <v>1.8109999999999999</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>73</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="3">
         <v>0.12</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="10">
+      <c r="C43" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="5">
         <v>15.89</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="E43" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="7">
         <v>7.95</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>74</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="3">
         <v>0.12</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="5">
+        <v>3.55</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="5">
+        <v>1.4430000000000001</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1562,22 +1603,22 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="27.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="178.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="27.7109375" style="3"/>
+    <col min="1" max="1" width="29.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="178.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="27.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1609,26 +1650,26 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>200</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>2</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>9</v>
       </c>
       <c r="H2" s="3">
@@ -1637,30 +1678,30 @@
       <c r="I2" s="3">
         <v>2.2593000000000001</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>700</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>2</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>16</v>
       </c>
       <c r="H3" s="3">
@@ -1669,30 +1710,30 @@
       <c r="I3" s="3">
         <v>3.2532999999999999</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>63</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>7.4</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>16.399999999999999</v>
       </c>
       <c r="H4" s="3">
@@ -1702,501 +1743,501 @@
       <c r="I4" s="3">
         <v>2.57</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="3">
         <v>108</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="14">
         <v>2</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="14">
         <v>6.5</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="15">
         <v>3.3000000000000003E-5</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="16">
         <v>2.6458651999999998</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E6" s="3">
         <v>113</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="14">
         <v>2.1</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="14">
         <v>7.5</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="15">
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="16">
         <v>2.8256119000000002</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E7" s="3">
         <v>25</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="14">
         <v>2.1</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="14">
         <v>5.9</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="15">
         <v>3.1699999999999998E-5</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="16">
         <v>2.4761397999999999</v>
       </c>
-      <c r="J7" s="25" t="s">
+      <c r="J7" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E8" s="3">
         <v>57</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="14">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="14">
         <v>7.8</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="15">
         <v>4.4299999999999999E-5</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="16">
         <v>2.202537</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="3">
         <v>196</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="14">
         <v>2.1</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="14">
         <v>6.2</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="15">
         <v>2.3900000000000002E-5</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="16">
         <v>2.7388843999999999</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E10" s="3">
         <v>367</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="14">
         <v>1.9</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="14">
         <v>10.199999999999999</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="15">
         <v>2.0999999999999999E-5</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="16">
         <v>2.8963214000000002</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E11" s="3">
         <v>599</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="14">
         <v>2.1</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="14">
         <v>9.6999999999999993</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="15">
         <v>2.2500000000000001E-5</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="16">
         <v>2.7443140000000001</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E12" s="3">
         <v>156</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="14">
         <v>2</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="14">
         <v>6.5</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="15">
         <v>3.0700000000000001E-5</v>
       </c>
-      <c r="I12" s="24">
+      <c r="I12" s="16">
         <v>2.6305483999999999</v>
       </c>
-      <c r="J12" s="25" t="s">
+      <c r="J12" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E13" s="3">
         <v>292</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="14">
         <v>2.1</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="14">
         <v>7.8</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="15">
         <v>1.9899999999999999E-5</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="16">
         <v>2.8436471000000001</v>
       </c>
-      <c r="J13" s="25" t="s">
+      <c r="J13" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E14" s="3">
         <v>37</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="14">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="14">
         <v>5.5</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="15">
         <v>9.3000000000000007E-6</v>
       </c>
-      <c r="I14" s="24">
+      <c r="I14" s="16">
         <v>3.2843296999999998</v>
       </c>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E15" s="3">
         <v>209</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="14">
         <v>1.9</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="14">
         <v>10.199999999999999</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="15">
         <v>1.63E-5</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15" s="16">
         <v>3.0492894000000001</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="J15" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E16" s="3">
         <v>307</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="14">
         <v>2.1</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="14">
         <v>9.6999999999999993</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="15">
         <v>2.51E-5</v>
       </c>
-      <c r="I16" s="24">
+      <c r="I16" s="16">
         <v>2.6718519000000001</v>
       </c>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E17" s="3">
         <v>84</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="14">
         <v>2</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="14">
         <v>10.199999999999999</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="15">
         <v>1.2E-5</v>
       </c>
-      <c r="I17" s="24">
+      <c r="I17" s="16">
         <v>3.2246939999999999</v>
       </c>
-      <c r="J17" s="25" t="s">
+      <c r="J17" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E18" s="3">
         <v>106</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="14">
         <v>3.3</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="14">
         <v>9.6999999999999993</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="15">
         <v>7.4000000000000003E-6</v>
       </c>
-      <c r="I18" s="24">
+      <c r="I18" s="16">
         <v>3.2745017999999999</v>
       </c>
-      <c r="J18" s="25" t="s">
+      <c r="J18" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E19" s="3">
         <v>39</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="14">
         <v>1.9</v>
       </c>
-      <c r="G19" s="22">
-        <v>10</v>
-      </c>
-      <c r="H19" s="23">
+      <c r="G19" s="14">
+        <v>10</v>
+      </c>
+      <c r="H19" s="15">
         <v>3.3399999999999999E-5</v>
       </c>
-      <c r="I19" s="24">
+      <c r="I19" s="16">
         <v>2.5935991999999999</v>
       </c>
-      <c r="J19" s="25" t="s">
+      <c r="J19" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E20" s="3">
@@ -2208,27 +2249,27 @@
       <c r="G20" s="3">
         <v>9.5</v>
       </c>
-      <c r="H20" s="23">
+      <c r="H20" s="15">
         <v>1.1600000000000001E-5</v>
       </c>
-      <c r="I20" s="24">
+      <c r="I20" s="16">
         <v>3.0595469</v>
       </c>
-      <c r="J20" s="25" t="s">
+      <c r="J20" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="3">
@@ -2237,103 +2278,103 @@
       <c r="F21" s="3">
         <v>2.9</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="14">
         <v>11</v>
       </c>
-      <c r="H21" s="23">
+      <c r="H21" s="15">
         <v>5.4E-6</v>
       </c>
-      <c r="I21" s="24">
+      <c r="I21" s="16">
         <v>3.2323621999999999</v>
       </c>
-      <c r="J21" s="25" t="s">
+      <c r="J21" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E22" s="3">
         <v>109</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="14">
         <v>2.1</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="14">
         <v>4.3</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H22" s="15">
         <v>1.7399999999999999E-5</v>
       </c>
-      <c r="I22" s="24">
+      <c r="I22" s="16">
         <v>2.8712141999999998</v>
       </c>
-      <c r="J22" s="25" t="s">
+      <c r="J22" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E23" s="3">
         <v>19</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="14">
         <v>2</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="14">
         <v>5.0999999999999996</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="15">
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="I23" s="24">
+      <c r="I23" s="16">
         <v>2.6410646999999998</v>
       </c>
-      <c r="J23" s="25" t="s">
+      <c r="J23" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>63</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>7.4</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>16.399999999999999</v>
       </c>
       <c r="H24" s="3">
@@ -2343,7 +2384,7 @@
       <c r="I24" s="3">
         <v>3.45</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="11" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>